<commit_message>
Modify the chute parts to slide into the t-slots rather than use fasteners
</commit_message>
<xml_diff>
--- a/Ackbar BOM.xlsx
+++ b/Ackbar BOM.xlsx
@@ -31,31 +31,31 @@
     <t>PETG Plastic (KG)</t>
   </si>
   <si>
-    <t>https://atomicfilament.com/products/deep-black-opaque-petg-pro</t>
-  </si>
-  <si>
-    <t>24" ABS Pipe 4" Diameter</t>
-  </si>
-  <si>
-    <t>https://www.homedepot.com/p/VPC-4-in-x-24-in-Plastic-ABS-Pipe-1204/202300521</t>
+    <t>https://www.amazon.com/dp/B0BN4Y1G2S/</t>
+  </si>
+  <si>
+    <t>ABS Pipe 4" Diameter 380mm length</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/VPC-4-in-x-10-ft-ABS-Cell-Core-Pipe-29-410HD/309282462</t>
   </si>
   <si>
     <t>ESP32-S3 Pico</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0BYJV4RWY</t>
+    <t>https://www.waveshare.com/product/mcu-tools/development-boards/esp32/esp32-s3-pico.htm</t>
   </si>
   <si>
     <t>E-Ink 1.54</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0728BJTZC</t>
+    <t>https://www.waveshare.com/product/displays/e-paper/epaper-3/1.54inch-e-paper-module.htm</t>
   </si>
   <si>
     <t>TMC2209</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B07ZQ3C1XW</t>
+    <t>https://www.amazon.com/dp/B0C373SJLQ/</t>
   </si>
   <si>
     <t>VL53L0X</t>
@@ -91,7 +91,7 @@
     <t>NEMA17 Stepper</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0B93HTR87</t>
+    <t>https://www.amazon.com/dp/B0B93LJPG2</t>
   </si>
   <si>
     <t>380mm 2020 Extrusion</t>
@@ -100,25 +100,25 @@
     <t>https://www.amazon.com/dp/B08KQCHTZL</t>
   </si>
   <si>
-    <t>M2.5 x 6mm</t>
+    <t>M2.5 x 6mm Socket Cap</t>
   </si>
   <si>
     <t>https://www.amazon.com/dp/B01H2108EW</t>
   </si>
   <si>
-    <t>M3 x 5mm</t>
+    <t>M3 x 5mm Socket Cap</t>
   </si>
   <si>
     <t>https://www.amazon.com/dp/B08B1T4HHP</t>
   </si>
   <si>
-    <t>M3 x 10mm</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B0BCG79KG4</t>
-  </si>
-  <si>
-    <t>M5 x 10mm</t>
+    <t>M3 x 20mm Socket Cap</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Socket-Screws-Metric-Stainless-Machine/dp/B0BM5L4NLF</t>
+  </si>
+  <si>
+    <t>M5 x 10mm Button Head</t>
   </si>
   <si>
     <t>https://www.amazon.com/dp/B0BKZ7WZFR</t>
@@ -158,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -211,6 +211,11 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Google Sans Mono&quot;"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -232,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -254,6 +259,7 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -481,7 +487,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.75"/>
+    <col customWidth="1" min="1" max="1" width="31.5"/>
     <col customWidth="1" min="5" max="5" width="71.0"/>
   </cols>
   <sheetData>
@@ -517,11 +523,11 @@
         <v>1.5</v>
       </c>
       <c r="C3" s="3">
-        <v>32.99</v>
+        <v>19.79</v>
       </c>
       <c r="D3" s="4">
         <f>PRODUCT(B3:C3)</f>
-        <v>49.485</v>
+        <v>29.685</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>6</v>
@@ -542,11 +548,11 @@
         <v>1.0</v>
       </c>
       <c r="C5" s="3">
-        <v>21.71</v>
+        <v>8.81</v>
       </c>
       <c r="D5" s="4">
         <f>PRODUCT(B5:C5)</f>
-        <v>21.71</v>
+        <v>8.81</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
@@ -567,11 +573,11 @@
         <v>1.0</v>
       </c>
       <c r="C7" s="3">
-        <v>16.99</v>
+        <v>10.99</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D25" si="1">PRODUCT(B7:C7)</f>
-        <v>16.99</v>
+        <f t="shared" ref="D7:D15" si="1">PRODUCT(B7:C7)</f>
+        <v>10.99</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
@@ -585,11 +591,11 @@
         <v>1.0</v>
       </c>
       <c r="C8" s="3">
-        <v>19.99</v>
+        <v>11.99</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="1"/>
-        <v>19.99</v>
+        <v>11.99</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>12</v>
@@ -603,11 +609,11 @@
         <v>1.0</v>
       </c>
       <c r="C9" s="3">
-        <v>5.4</v>
+        <v>3.75</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>5.4</v>
+        <v>3.75</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>14</v>
@@ -711,204 +717,214 @@
         <v>1.0</v>
       </c>
       <c r="C15" s="3">
-        <v>11.99</v>
+        <v>9.99</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="1"/>
-        <v>11.99</v>
+        <v>9.99</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>3.12</v>
-      </c>
-      <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>12.48</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C17" s="3">
-        <v>0.0759</v>
+        <v>3.12</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1518</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>30</v>
+        <f t="shared" ref="D17:D26" si="2">PRODUCT(B17:C17)</f>
+        <v>12.48</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C18" s="3">
-        <v>0.0788</v>
+        <v>0.0759</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4728</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>32</v>
+        <f t="shared" si="2"/>
+        <v>0.1518</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="C19" s="3">
-        <v>0.0828</v>
+        <v>0.0788</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3312</v>
+        <f t="shared" si="2"/>
+        <v>0.788</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="3">
-        <v>22.0</v>
+        <v>6.0</v>
       </c>
       <c r="C20" s="3">
         <v>0.0939</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="1"/>
-        <v>2.0658</v>
+        <f t="shared" si="2"/>
+        <v>0.5634</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="C21" s="3">
-        <v>0.1898</v>
+        <v>0.0939</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="1"/>
-        <v>1.898</v>
+        <f t="shared" si="2"/>
+        <v>1.1268</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="C22" s="3">
-        <v>0.333</v>
+        <v>0.1898</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="1"/>
-        <v>1.332</v>
+        <f t="shared" si="2"/>
+        <v>1.5184</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3">
-        <v>22.0</v>
+        <v>4.0</v>
       </c>
       <c r="C23" s="3">
-        <v>0.1598</v>
-      </c>
-      <c r="D23" s="7">
-        <f t="shared" si="1"/>
-        <v>3.5156</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>42</v>
+        <v>0.333</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="2"/>
+        <v>1.332</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B24" s="3">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="C24" s="3">
-        <v>0.11</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="1"/>
-        <v>0.22</v>
+        <v>0.1598</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="2"/>
+        <v>1.9176</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="3">
         <v>12.0</v>
       </c>
       <c r="C25" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="2"/>
+        <v>1.32</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="C26" s="3">
         <v>0.26</v>
       </c>
-      <c r="D25" s="4">
-        <f t="shared" si="1"/>
+      <c r="D26" s="4">
+        <f t="shared" si="2"/>
         <v>3.12</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27">
-      <c r="D27" s="8">
-        <f>SUM(D3:D25)</f>
-        <v>168.2122</v>
-      </c>
+    <row r="28">
+      <c r="D28" s="8">
+        <f>SUM(D3:D26)</f>
+        <v>116.593</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" s="9"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
@@ -925,16 +941,16 @@
     <hyperlink r:id="rId9" ref="E13"/>
     <hyperlink r:id="rId10" ref="E14"/>
     <hyperlink r:id="rId11" ref="E15"/>
-    <hyperlink r:id="rId12" ref="E16"/>
-    <hyperlink r:id="rId13" ref="E17"/>
-    <hyperlink r:id="rId14" ref="E18"/>
-    <hyperlink r:id="rId15" ref="E19"/>
-    <hyperlink r:id="rId16" ref="E20"/>
-    <hyperlink r:id="rId17" ref="E21"/>
-    <hyperlink r:id="rId18" ref="E22"/>
-    <hyperlink r:id="rId19" ref="E23"/>
-    <hyperlink r:id="rId20" ref="E24"/>
-    <hyperlink r:id="rId21" ref="E25"/>
+    <hyperlink r:id="rId12" ref="E17"/>
+    <hyperlink r:id="rId13" ref="E18"/>
+    <hyperlink r:id="rId14" ref="E19"/>
+    <hyperlink r:id="rId15" ref="E20"/>
+    <hyperlink r:id="rId16" ref="E21"/>
+    <hyperlink r:id="rId17" ref="E22"/>
+    <hyperlink r:id="rId18" ref="E23"/>
+    <hyperlink r:id="rId19" ref="E24"/>
+    <hyperlink r:id="rId20" ref="E25"/>
+    <hyperlink r:id="rId21" ref="E26"/>
   </hyperlinks>
   <drawing r:id="rId22"/>
 </worksheet>

</xml_diff>